<commit_message>
Reorganize test data with sales_tax and use_tax folders
- Add new test_data/sales_tax/ and test_data/use_tax/ with organized invoice/PO files
- Update synthetic Excel claims with new test rows
- Remove old test_data/invoices/ and test_data/purchase_orders/
- Add test data generation and sync scripts

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/test_data/synthetic/SalesTax_Claims - Analyzed.xlsx
+++ b/test_data/synthetic/SalesTax_Claims - Analyzed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="284">
   <si>
     <t>Vendor ID</t>
   </si>
@@ -145,6 +145,18 @@
     <t>V0020</t>
   </si>
   <si>
+    <t>V0021</t>
+  </si>
+  <si>
+    <t>V0022</t>
+  </si>
+  <si>
+    <t>V0023</t>
+  </si>
+  <si>
+    <t>V0024</t>
+  </si>
+  <si>
     <t>Lake Systems Group</t>
   </si>
   <si>
@@ -184,6 +196,9 @@
     <t>River Analytics LLC</t>
   </si>
   <si>
+    <t>Northstar Technologies Inc</t>
+  </si>
+  <si>
     <t>INV-2024-10001.pdf</t>
   </si>
   <si>
@@ -271,6 +286,18 @@
     <t>PO-4900100009.pdf</t>
   </si>
   <si>
+    <t>PO-Equipment-Tracker.xlsx</t>
+  </si>
+  <si>
+    <t>PO-License-Summary.xlsx</t>
+  </si>
+  <si>
+    <t>PO-Request-Email.eml</t>
+  </si>
+  <si>
+    <t>PO-Service-Quotation.docx</t>
+  </si>
+  <si>
     <t>INV-2024-10001</t>
   </si>
   <si>
@@ -331,6 +358,12 @@
     <t>INV-2024-10020</t>
   </si>
   <si>
+    <t>PO-4900596750</t>
+  </si>
+  <si>
+    <t>Q-78146</t>
+  </si>
+  <si>
     <t>2023-01-26</t>
   </si>
   <si>
@@ -424,6 +457,12 @@
     <t>Development Tools Package, Cloud Platform Access</t>
   </si>
   <si>
+    <t>IT Equipment (Multi-vendor PO)</t>
+  </si>
+  <si>
+    <t>Software License (Multi-vendor PO)</t>
+  </si>
+  <si>
     <t>2x Analytics Platform Subscription ($45,741.00 ea), 10x Enterprise License - Annual Subscription ($42,651.00 ea)</t>
   </si>
   <si>
@@ -484,6 +523,18 @@
     <t>7x Professional Services - Implementation ($673,141.00 total)</t>
   </si>
   <si>
+    <t>Cloud Platform Access, Network Switch, Technical Consulting, Server Rack, Managed Services</t>
+  </si>
+  <si>
+    <t>System Integration, Training Program, Storage Array, Professional Services, Security Suite</t>
+  </si>
+  <si>
+    <t>Workstation - High Performance (5), Network Switch - 48 Port (4), UPS Battery Backup System (3)</t>
+  </si>
+  <si>
+    <t>Data services implementation</t>
+  </si>
+  <si>
     <t>INVOICE Lake Systems Group 600 Automotive Way Detroit, MI 48201 Tax ID: 38-1234560 Phone: (313) 555-1200 PLEASE REFER TO YOUR ACCOUNT NO., AND OUR INVOICE AND ORDER NO. IN ALL COMMUNICATIONS REGARDING THIS INVOICE</t>
   </si>
   <si>
@@ -592,37 +643,58 @@
     <t>SFT-DEV-005, SFT-CLD-002</t>
   </si>
   <si>
+    <t>Equipment Tracker, Multi-vendor</t>
+  </si>
+  <si>
+    <t>License Summary, Multi-vendor</t>
+  </si>
+  <si>
+    <t>Workstation, Network Switch, UPS</t>
+  </si>
+  <si>
+    <t>Professional Services Quotation</t>
+  </si>
+  <si>
+    <t>Software Subscription - Enterprise</t>
+  </si>
+  <si>
+    <t>Professional Services - IT Consulting</t>
+  </si>
+  <si>
+    <t>Hardware - Server Rack</t>
+  </si>
+  <si>
+    <t>Software License - Database Management System</t>
+  </si>
+  <si>
+    <t>Professional Services - Support Contract</t>
+  </si>
+  <si>
+    <t>Professional Services - Network Infrastructure Design</t>
+  </si>
+  <si>
+    <t>Hardware - IT Equipment</t>
+  </si>
+  <si>
+    <t>Software License - Enterprise</t>
+  </si>
+  <si>
     <t>Software Subscription - SaaS</t>
   </si>
   <si>
-    <t>Professional Services - IT Consulting</t>
-  </si>
-  <si>
-    <t>IT Equipment - Hardware</t>
-  </si>
-  <si>
-    <t>Electronic Software Delivery - Software License</t>
-  </si>
-  <si>
-    <t>Software License - Enterprise</t>
-  </si>
-  <si>
-    <t>Professional Services - Technical Support</t>
-  </si>
-  <si>
-    <t>Hardware - IT Equipment</t>
-  </si>
-  <si>
-    <t>Professional Services - Technical Consulting</t>
-  </si>
-  <si>
-    <t>SaaS Subscription</t>
-  </si>
-  <si>
     <t>Hardware - Network Equipment</t>
   </si>
   <si>
-    <t>Software License - Cloud Platform Access</t>
+    <t>Software License - Cloud Platform</t>
+  </si>
+  <si>
+    <t>Tangible Personal Property - IT Equipment</t>
+  </si>
+  <si>
+    <t>Software License - Multi-vendor</t>
+  </si>
+  <si>
+    <t>Professional Services - Data Services Implementation</t>
   </si>
   <si>
     <t>MPU</t>
@@ -634,18 +706,21 @@
     <t>No Refund</t>
   </si>
   <si>
+    <t>Wrong Rate</t>
+  </si>
+  <si>
     <t>WAC 458-20-15502</t>
   </si>
   <si>
     <t>WAC 458-20-224</t>
   </si>
   <si>
-    <t>WAC 458-20-178</t>
-  </si>
-  <si>
     <t>WAC 458-20-155</t>
   </si>
   <si>
+    <t>WAC 458-20-145</t>
+  </si>
+  <si>
     <t>WAC 458-20-15501</t>
   </si>
   <si>
@@ -661,6 +736,9 @@
     <t>80%</t>
   </si>
   <si>
+    <t>60%</t>
+  </si>
+  <si>
     <t>75%</t>
   </si>
   <si>
@@ -700,9 +778,6 @@
     <t>$34,115.14</t>
   </si>
   <si>
-    <t>$517.71</t>
-  </si>
-  <si>
     <t>$50,367.44</t>
   </si>
   <si>
@@ -712,70 +787,94 @@
     <t>$55,534.13</t>
   </si>
   <si>
-    <t>The transaction involves a software subscription, likely SaaS, which qualifies for the MPU refund basis as it is used at multiple locations. This aligns with historical patterns for software licenses. The refund is calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>Professional services, primarily human effort, are generally non-taxable in Washington State. The transaction involves IT consulting and training, which are non-taxable services under WAC 458-20-224.</t>
-  </si>
-  <si>
-    <t>The transaction involves tangible personal property (IT equipment), which is taxable in Washington State. No refund is applicable as hardware is not eligible for MPU or other exemptions.</t>
-  </si>
-  <si>
-    <t>The transaction involves electronic software delivery, qualifying for the MPU refund basis as it is likely used at multiple locations. This aligns with historical patterns for software licenses. The refund is calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>The transaction involves a software license, likely used at multiple locations, qualifying for the MPU refund basis. This aligns with historical patterns for software licenses. The refund is calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>Professional services primarily involving human effort, such as consulting and training, are generally not subject to sales tax in Washington State. Based on WAC 458-20-224, these services are non-taxable. The vendor's business type and service descriptions align with this classification.</t>
-  </si>
-  <si>
-    <t>Technical support services are considered professional services and are primarily human effort, which are non-taxable under WAC 458-20-224. The vendor's description supports this classification.</t>
-  </si>
-  <si>
-    <t>The services provided by Coastal Networks Inc. are categorized as professional services, which are non-taxable under Washington State law (WAC 458-20-224). The nature of the services aligns with this classification.</t>
-  </si>
-  <si>
-    <t>Software licenses used at multiple locations qualify for the MPU exemption under WAC 458-20-15502. The vendor's business type and product description suggest applicability of MPU.</t>
-  </si>
-  <si>
-    <t>IT equipment is tangible personal property and is taxable in Washington State. There is no basis for a refund as per WAC 458-20-155.</t>
-  </si>
-  <si>
-    <t>The transaction involves a software license, which is eligible for the MPU refund basis as it likely involves multiple points of use across different locations. According to WAC 458-20-15502, software licenses used in multiple locations can qualify for a tax refund under the MPU provision. The refund is calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>Professional services such as technical consulting are generally not subject to sales tax in Washington State as they primarily involve human effort. According to WAC 458-20-224, services that do not involve the sale of tangible personal property are exempt from sales tax. Therefore, the entire tax charged is refundable.</t>
-  </si>
-  <si>
-    <t>The transaction involves tangible personal property (IT equipment), which is taxable in Washington State. According to WAC 458-20-155, sales of tangible personal property are subject to sales tax. Therefore, no refund is applicable.</t>
-  </si>
-  <si>
-    <t>The transaction involves a software subscription, which is eligible for the MPU refund basis as it likely involves multiple points of use across different locations. According to WAC 458-20-15502, software subscriptions used in multiple locations can qualify for a tax refund under the MPU provision. The refund is calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>The transaction involves electronic software delivery, which is eligible for the MPU refund basis as it likely involves multiple points of use across different locations. According to WAC 458-20-15502, electronic software deliveries used in multiple locations can qualify for a tax refund under the MPU provision. The refund is calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>The transaction involves a software license, which is eligible for the MPU refund basis as it is likely used at multiple locations. According to WAC 458-20-15502, software licenses can qualify for MPU if used across multiple points. The vendor's business type supports this classification. Refund calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>The transaction involves tangible personal property, specifically IT equipment, which is taxable in Washington State. According to WAC 458-20-15501, tangible personal property is subject to sales tax. No refund is applicable.</t>
-  </si>
-  <si>
-    <t>The transaction involves tangible personal property, specifically network equipment, which is taxable in Washington State. According to WAC 458-20-15501, tangible personal property is subject to sales tax. No refund is applicable.</t>
-  </si>
-  <si>
-    <t>The transaction involves a cloud platform access, which is considered a software license and eligible for the MPU refund basis if used at multiple locations. According to WAC 458-20-15502, software licenses can qualify for MPU. Refund calculated as 80% of the tax charged.</t>
-  </si>
-  <si>
-    <t>The transaction involves professional services, which are generally non-taxable if they primarily involve human effort. According to WAC 458-20-224, professional services are exempt from sales tax. Full refund of the tax charged is applicable.</t>
+    <t>$55,107.01</t>
+  </si>
+  <si>
+    <t>$1,157.28</t>
+  </si>
+  <si>
+    <t>$46,335.97</t>
+  </si>
+  <si>
+    <t>The transaction involves a software subscription, which is classified under software licenses. According to WAC 458-20-15502, software licenses used at multiple locations qualify for MPU. The refund is calculated as 80% of the tax paid, as per MPU rules.</t>
+  </si>
+  <si>
+    <t>Professional services primarily involving human effort are generally non-taxable under WAC 458-20-224. The services provided include consulting and training, which fall under this exemption. Therefore, the entire tax paid is refundable.</t>
+  </si>
+  <si>
+    <t>The transaction involves tangible personal property (server racks), which is taxable in Washington State as per WAC 458-20-155. No refund is applicable as the tax was correctly applied to tangible personal property.</t>
+  </si>
+  <si>
+    <t>The transaction involves electronic software delivery, which qualifies for MPU under WAC 458-20-15502 if used at multiple locations. The refund is 80% of the tax paid, consistent with MPU rules.</t>
+  </si>
+  <si>
+    <t>The transaction involves a software license, which is eligible for MPU under WAC 458-20-15502 if used at multiple locations. The refund is calculated as 80% of the tax paid, following MPU guidelines.</t>
+  </si>
+  <si>
+    <t>Professional services, such as IT consulting, are generally not subject to sales tax in Washington State as they are primarily human effort. Therefore, the entire tax paid is eligible for refund.</t>
+  </si>
+  <si>
+    <t>Support contracts, when classified as professional services, are not taxable in Washington State. The tax paid on this transaction is eligible for a full refund.</t>
+  </si>
+  <si>
+    <t>Professional services related to network infrastructure design are not taxable in Washington State. The tax paid on this transaction is eligible for a full refund.</t>
+  </si>
+  <si>
+    <t>Software licenses used at multiple locations may qualify for the Multiple Points of Use (MPU) exemption. 80% of the tax paid is eligible for refund.</t>
+  </si>
+  <si>
+    <t>IT equipment is considered tangible personal property and is taxable in Washington State. No refund is applicable for this transaction.</t>
+  </si>
+  <si>
+    <t>The product is classified as a software license, which is eligible for MPU treatment under WAC 458-20-15502. The vendor is a software company, and the description suggests enterprise software, which aligns with historical patterns for MPU refunds.</t>
+  </si>
+  <si>
+    <t>The services provided are primarily human effort, such as consulting and support, which are non-taxable under WAC 458-20-224. This aligns with historical patterns for non-taxable service refunds.</t>
+  </si>
+  <si>
+    <t>The transaction involves tangible personal property, specifically IT equipment, which is taxable in Washington under WAC 458-20-145. No refund is applicable.</t>
+  </si>
+  <si>
+    <t>The product is a software subscription, likely SaaS, which qualifies for MPU under WAC 458-20-15502. The vendor's business type supports this classification, consistent with historical refund patterns.</t>
+  </si>
+  <si>
+    <t>The transaction includes hardware items, such as a workstation and server rack, which are taxable as tangible personal property under WAC 458-20-15502. Despite the vendor's software distribution context, the items are physical, leading to no refund.</t>
+  </si>
+  <si>
+    <t>The transaction involves a software license, which is eligible for MPU treatment as it likely involves multiple points of use across different locations. Under WAC 458-20-15502, software licenses used at multiple locations can be apportioned for tax purposes. The refund is calculated as 80% of the tax paid, which is $62,959.30 * 0.80 = $50,367.44.</t>
+  </si>
+  <si>
+    <t>The transaction involves tangible personal property (IT equipment), which is taxable in Washington State. According to WAC 458-20-15501, tangible personal property is subject to sales tax. Therefore, no refund is applicable.</t>
+  </si>
+  <si>
+    <t>The transaction involves tangible personal property (network equipment), which is taxable in Washington State. According to WAC 458-20-15501, tangible personal property is subject to sales tax. Therefore, no refund is applicable.</t>
+  </si>
+  <si>
+    <t>The transaction involves a software license for cloud platform access, which is eligible for MPU treatment as it likely involves multiple points of use across different locations. Under WAC 458-20-15502, software licenses used at multiple locations can be apportioned for tax purposes. The refund is calculated as 80% of the tax paid, which is $5,538.75 * 0.80 = $4,431.00.</t>
+  </si>
+  <si>
+    <t>The transaction involves professional services, which are generally non-taxable in Washington State if they primarily involve human effort. According to WAC 458-20-224, professional services are exempt from sales tax. Therefore, the full amount of tax paid is eligible for refund.</t>
+  </si>
+  <si>
+    <t>The transaction involves tangible personal property (IT Equipment) which is taxable in Washington State. According to WAC 458-20-155, tangible personal property is subject to sales tax. Therefore, no refund is applicable.</t>
+  </si>
+  <si>
+    <t>The transaction involves a software license, which is eligible for MPU (Multiple Points of Use) treatment under WAC 458-20-15502. This allows for a refund of 80% of the tax paid if the software is used in multiple locations. The estimated refund amount is calculated as 80% of the tax charged.</t>
+  </si>
+  <si>
+    <t>The transaction involves tangible personal property (IT Equipment) which is taxable in Washington State. However, the tax rate applied was 6.0%, which is lower than the typical 8.0% rate for such items. This suggests a potential overcharge or wrong rate application. The estimated refund is based on the difference between the charged rate and the correct rate.</t>
+  </si>
+  <si>
+    <t>The transaction involves professional services, which are generally non-taxable in Washington State if they primarily involve human effort, as per WAC 458-20-224. Given the nature of the services (data services implementation), the entire tax paid is eligible for refund.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -828,11 +927,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1127,7 +1227,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1209,22 +1309,22 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G2">
         <v>4500256787</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I2">
         <v>517992</v>
@@ -1239,37 +1339,37 @@
         <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="N2" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P2" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q2" t="s">
         <v>136</v>
       </c>
-      <c r="O2" t="s">
-        <v>156</v>
-      </c>
-      <c r="P2" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>125</v>
-      </c>
       <c r="R2" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="S2" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T2" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U2" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="V2" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="W2" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -1277,22 +1377,22 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="G3">
         <v>4500243962</v>
       </c>
       <c r="H3" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="I3">
         <v>577078</v>
@@ -1307,37 +1407,37 @@
         <v>7.9</v>
       </c>
       <c r="M3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="N3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O3" t="s">
+        <v>174</v>
+      </c>
+      <c r="P3" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q3" t="s">
         <v>137</v>
       </c>
-      <c r="O3" t="s">
-        <v>157</v>
-      </c>
-      <c r="P3" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>126</v>
-      </c>
       <c r="R3" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="S3" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="T3" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="U3" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="V3" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="W3" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -1345,19 +1445,19 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="I4">
         <v>34902</v>
@@ -1372,37 +1472,37 @@
         <v>8.75</v>
       </c>
       <c r="M4" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="N4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4" t="s">
         <v>138</v>
       </c>
-      <c r="O4" t="s">
-        <v>158</v>
-      </c>
-      <c r="P4" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>127</v>
-      </c>
       <c r="R4" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="S4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="T4" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="U4" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="V4" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="W4" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -1410,22 +1510,22 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G5">
         <v>4500738797</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="I5">
         <v>317368</v>
@@ -1440,37 +1540,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="M5" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="N5" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" t="s">
+        <v>176</v>
+      </c>
+      <c r="P5" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q5" t="s">
         <v>139</v>
       </c>
-      <c r="O5" t="s">
-        <v>159</v>
-      </c>
-      <c r="P5" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>128</v>
-      </c>
       <c r="R5" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="S5" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T5" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U5" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="V5" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="W5" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1478,19 +1578,19 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="I6">
         <v>268960</v>
@@ -1505,37 +1605,37 @@
         <v>6</v>
       </c>
       <c r="M6" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="N6" t="s">
+        <v>153</v>
+      </c>
+      <c r="O6" t="s">
+        <v>177</v>
+      </c>
+      <c r="P6" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q6" t="s">
         <v>140</v>
       </c>
-      <c r="O6" t="s">
-        <v>160</v>
-      </c>
-      <c r="P6" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>129</v>
-      </c>
       <c r="R6" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="S6" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T6" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U6" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="V6" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="W6" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -1543,19 +1643,19 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="I7">
         <v>542640</v>
@@ -1570,37 +1670,37 @@
         <v>10.25</v>
       </c>
       <c r="M7" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="N7" t="s">
+        <v>154</v>
+      </c>
+      <c r="O7" t="s">
+        <v>178</v>
+      </c>
+      <c r="P7" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q7" t="s">
         <v>141</v>
       </c>
-      <c r="O7" t="s">
-        <v>161</v>
-      </c>
-      <c r="P7" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>130</v>
-      </c>
       <c r="R7" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="S7" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="T7" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="U7" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="V7" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="W7" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -1608,22 +1708,22 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>4500149811</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="I8">
         <v>89802</v>
@@ -1638,37 +1738,37 @@
         <v>5.6</v>
       </c>
       <c r="M8" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="N8" t="s">
+        <v>155</v>
+      </c>
+      <c r="O8" t="s">
+        <v>179</v>
+      </c>
+      <c r="P8" t="s">
         <v>142</v>
       </c>
-      <c r="O8" t="s">
-        <v>162</v>
-      </c>
-      <c r="P8" t="s">
-        <v>131</v>
-      </c>
       <c r="Q8" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="R8" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="S8" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="T8" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="U8" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="V8" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="W8" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -1676,19 +1776,19 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="I9">
         <v>1056168</v>
@@ -1703,37 +1803,37 @@
         <v>6.5</v>
       </c>
       <c r="M9" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="N9" t="s">
+        <v>156</v>
+      </c>
+      <c r="O9" t="s">
+        <v>180</v>
+      </c>
+      <c r="P9" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q9" t="s">
         <v>143</v>
       </c>
-      <c r="O9" t="s">
-        <v>163</v>
-      </c>
-      <c r="P9" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>132</v>
-      </c>
       <c r="R9" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="S9" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="T9" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="U9" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="V9" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="W9" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -1741,19 +1841,19 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="I10">
         <v>789482</v>
@@ -1768,37 +1868,37 @@
         <v>6</v>
       </c>
       <c r="M10" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="N10" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="O10" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="P10" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="Q10" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="R10" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="S10" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T10" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U10" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
       <c r="V10" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="W10" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -1806,19 +1906,19 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="G11">
         <v>4900963110</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="I11">
         <v>213852</v>
@@ -1833,37 +1933,37 @@
         <v>8.75</v>
       </c>
       <c r="M11" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="N11" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="O11" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="P11" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="Q11" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="R11" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="S11" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="T11" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="U11" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="V11" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="W11" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -1871,19 +1971,19 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G12">
         <v>4500921406</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="I12">
         <v>350312</v>
@@ -1898,37 +1998,37 @@
         <v>6.25</v>
       </c>
       <c r="M12" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="N12" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="O12" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="P12" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="Q12" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="R12" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="S12" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T12" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U12" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="V12" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="W12" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -1936,16 +2036,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="I13">
         <v>1470171</v>
@@ -1960,37 +2060,37 @@
         <v>7.88</v>
       </c>
       <c r="M13" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="N13" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="O13" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="P13" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="Q13" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="R13" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="S13" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="T13" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="U13" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="V13" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="W13" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -1998,19 +2098,19 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G14">
         <v>4900074441</v>
       </c>
       <c r="H14" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="I14">
         <v>323196</v>
@@ -2025,37 +2125,37 @@
         <v>7</v>
       </c>
       <c r="M14" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="N14" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="O14" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="P14" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="Q14" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="R14" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="S14" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="T14" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="U14" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="V14" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="W14" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -2063,19 +2163,19 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="G15">
         <v>4500074299</v>
       </c>
       <c r="H15" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="I15">
         <v>516896</v>
@@ -2090,37 +2190,37 @@
         <v>8.25</v>
       </c>
       <c r="M15" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="N15" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="O15" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="P15" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="Q15" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="R15" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="S15" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T15" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U15" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="V15" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="W15" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -2128,19 +2228,19 @@
         <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G16">
         <v>4500260735</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="I16">
         <v>11556</v>
@@ -2155,37 +2255,37 @@
         <v>5.6</v>
       </c>
       <c r="M16" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="N16" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="O16" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="P16" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="Q16" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="R16" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="S16" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c r="T16" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U16" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="V16" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="W16" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -2193,19 +2293,19 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G17">
         <v>4900146991</v>
       </c>
       <c r="H17" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="I17">
         <v>763143</v>
@@ -2220,37 +2320,37 @@
         <v>8.199999999999999</v>
       </c>
       <c r="M17" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="N17" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="O17" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="P17" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="Q17" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="R17" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="S17" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T17" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U17" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="V17" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="W17" t="s">
-        <v>247</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -2258,16 +2358,16 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="H18" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="I18">
         <v>63529</v>
@@ -2282,37 +2382,37 @@
         <v>6.25</v>
       </c>
       <c r="M18" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="N18" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="O18" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="P18" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="Q18" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="R18" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="S18" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="T18" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="U18" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="V18" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="W18" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -2320,19 +2420,19 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="G19">
         <v>4900052578</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="I19">
         <v>46157</v>
@@ -2347,37 +2447,37 @@
         <v>8.9</v>
       </c>
       <c r="M19" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="N19" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="O19" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="P19" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="Q19" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="R19" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="S19" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="T19" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="U19" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="V19" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="W19" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -2385,19 +2485,19 @@
         <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G20">
         <v>4900165080</v>
       </c>
       <c r="H20" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="I20">
         <v>88620</v>
@@ -2412,37 +2512,37 @@
         <v>6.2</v>
       </c>
       <c r="M20" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="N20" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="O20" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="P20" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="Q20" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="R20" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="S20" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="T20" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="U20" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="V20" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="W20" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -2450,16 +2550,16 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="H21" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="I21">
         <v>673141</v>
@@ -2474,37 +2574,267 @@
         <v>8.25</v>
       </c>
       <c r="M21" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="N21" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="O21" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="P21" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="Q21" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="R21" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="S21" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="T21" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="U21" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="V21" t="s">
+        <v>256</v>
+      </c>
+      <c r="W21" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="2">
+        <v>45200</v>
+      </c>
+      <c r="I22">
+        <v>154556</v>
+      </c>
+      <c r="J22">
+        <v>12364.48</v>
+      </c>
+      <c r="K22">
+        <v>166920.48</v>
+      </c>
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22" t="s">
+        <v>147</v>
+      </c>
+      <c r="N22" t="s">
+        <v>169</v>
+      </c>
+      <c r="P22" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>147</v>
+      </c>
+      <c r="R22" t="s">
+        <v>224</v>
+      </c>
+      <c r="S22" t="s">
+        <v>229</v>
+      </c>
+      <c r="T22" t="s">
+        <v>233</v>
+      </c>
+      <c r="U22" t="s">
+        <v>237</v>
+      </c>
+      <c r="V22" t="s">
+        <v>244</v>
+      </c>
+      <c r="W22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="2">
+        <v>45476</v>
+      </c>
+      <c r="I23">
+        <v>861047</v>
+      </c>
+      <c r="J23">
+        <v>68883.75999999999</v>
+      </c>
+      <c r="K23">
+        <v>929930.76</v>
+      </c>
+      <c r="L23">
+        <v>8</v>
+      </c>
+      <c r="M23" t="s">
+        <v>148</v>
+      </c>
+      <c r="N23" t="s">
+        <v>170</v>
+      </c>
+      <c r="P23" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>148</v>
+      </c>
+      <c r="R23" t="s">
+        <v>225</v>
+      </c>
+      <c r="S23" t="s">
+        <v>227</v>
+      </c>
+      <c r="T23" t="s">
         <v>231</v>
       </c>
-      <c r="W21" t="s">
-        <v>251</v>
+      <c r="U23" t="s">
+        <v>236</v>
+      </c>
+      <c r="V23" t="s">
+        <v>257</v>
+      </c>
+      <c r="W23" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="2">
+        <v>45345</v>
+      </c>
+      <c r="I24">
+        <v>57864</v>
+      </c>
+      <c r="J24">
+        <v>3471.84</v>
+      </c>
+      <c r="K24">
+        <v>61335.84</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24" t="s">
+        <v>138</v>
+      </c>
+      <c r="N24" t="s">
+        <v>171</v>
+      </c>
+      <c r="P24" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>138</v>
+      </c>
+      <c r="R24" t="s">
+        <v>224</v>
+      </c>
+      <c r="S24" t="s">
+        <v>230</v>
+      </c>
+      <c r="T24" t="s">
+        <v>234</v>
+      </c>
+      <c r="U24" t="s">
+        <v>239</v>
+      </c>
+      <c r="V24" t="s">
+        <v>258</v>
+      </c>
+      <c r="W24" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="2">
+        <v>44928</v>
+      </c>
+      <c r="I25">
+        <v>827428</v>
+      </c>
+      <c r="J25">
+        <v>46335.97</v>
+      </c>
+      <c r="K25">
+        <v>873763.97</v>
+      </c>
+      <c r="L25">
+        <v>5.6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>143</v>
+      </c>
+      <c r="N25" t="s">
+        <v>172</v>
+      </c>
+      <c r="P25" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>143</v>
+      </c>
+      <c r="R25" t="s">
+        <v>226</v>
+      </c>
+      <c r="S25" t="s">
+        <v>228</v>
+      </c>
+      <c r="T25" t="s">
+        <v>232</v>
+      </c>
+      <c r="U25" t="s">
+        <v>241</v>
+      </c>
+      <c r="V25" t="s">
+        <v>259</v>
+      </c>
+      <c r="W25" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>